<commit_message>
Updated activity data for custom table case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/IFRS9_Stage3/ActivityData/ActivityData_D2.xlsx
+++ b/src/test/resources/TestDriver/IFRS9_Stage3/ActivityData/ActivityData_D2.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\IFRS9_Stage3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\fyntrac-data-main\fyntrac-data-main\src\test\resources\TestDriver\IFRS9_Stage3\ActivityData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AF1F3F-D91A-49A4-AAB8-C4E25E315281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2F958A-2F64-4853-96F6-BF837F2B04EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpectedCashFlow" sheetId="9" r:id="rId1"/>
-    <sheet name="GLRule" sheetId="7" state="hidden" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="8" state="hidden" r:id="rId3"/>
+    <sheet name="MeasurementType" sheetId="10" r:id="rId2"/>
+    <sheet name="GLRule" sheetId="7" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="8" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="44">
   <si>
     <t>PostingDate</t>
   </si>
@@ -148,9 +149,6 @@
     <t>Attributeid</t>
   </si>
   <si>
-    <t>ImpairmentType</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
@@ -164,13 +162,22 @@
   </si>
   <si>
     <t>LN-1002</t>
+  </si>
+  <si>
+    <t>MeasurementType</t>
+  </si>
+  <si>
+    <t>Collateral</t>
+  </si>
+  <si>
+    <t>FairValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +207,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -241,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -250,6 +264,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842CF9C8-9C33-44D4-B175-3D20CAE2D3CA}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,13 +558,13 @@
         <v>35</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -560,13 +575,13 @@
         <v>45716</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="7">
         <v>45716</v>
@@ -583,13 +598,13 @@
         <v>45716</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="7">
         <v>45747</v>
@@ -606,13 +621,13 @@
         <v>45716</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="7">
         <v>45777</v>
@@ -629,13 +644,13 @@
         <v>45716</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7">
         <v>45808</v>
@@ -652,13 +667,13 @@
         <v>45716</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="7">
         <v>45838</v>
@@ -675,13 +690,13 @@
         <v>45716</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7">
         <v>45869</v>
@@ -698,13 +713,13 @@
         <v>45716</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7">
         <v>45900</v>
@@ -721,13 +736,13 @@
         <v>45716</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7">
         <v>45930</v>
@@ -744,13 +759,13 @@
         <v>45716</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="7">
         <v>45961</v>
@@ -767,13 +782,13 @@
         <v>45716</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="7">
         <v>45991</v>
@@ -790,13 +805,13 @@
         <v>45716</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="7">
         <v>46022</v>
@@ -813,13 +828,13 @@
         <v>45716</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="7">
         <v>46053</v>
@@ -836,13 +851,13 @@
         <v>45716</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="7">
         <v>45716</v>
@@ -859,13 +874,13 @@
         <v>45716</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="7">
         <v>45747</v>
@@ -882,13 +897,13 @@
         <v>45716</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="7">
         <v>45777</v>
@@ -905,13 +920,13 @@
         <v>45716</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="7">
         <v>45808</v>
@@ -928,13 +943,13 @@
         <v>45716</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="7">
         <v>45838</v>
@@ -951,13 +966,13 @@
         <v>45716</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="7">
         <v>45869</v>
@@ -974,13 +989,13 @@
         <v>45716</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="7">
         <v>45900</v>
@@ -997,13 +1012,13 @@
         <v>45716</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="7">
         <v>45930</v>
@@ -1020,13 +1035,13 @@
         <v>45716</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F22" s="7">
         <v>45961</v>
@@ -1043,13 +1058,13 @@
         <v>45716</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="7">
         <v>45991</v>
@@ -1066,13 +1081,13 @@
         <v>45716</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="7">
         <v>46022</v>
@@ -1089,13 +1104,13 @@
         <v>45716</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="7">
         <v>46053</v>
@@ -1110,6 +1125,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B65EE7-6F2F-45F0-9B70-77809783DC5E}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1417,7 +1471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:O25"/>
   <sheetViews>

</xml_diff>